<commit_message>
finish upload excel - need test
</commit_message>
<xml_diff>
--- a/StoreManagement.Website/Resource/ImportedTemplate/Products.xlsx
+++ b/StoreManagement.Website/Resource/ImportedTemplate/Products.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>VAT</t>
   </si>
@@ -67,6 +67,30 @@
   </si>
   <si>
     <t>Quản lý thuộc tính?</t>
+  </si>
+  <si>
+    <t>Áo thun BB - S</t>
+  </si>
+  <si>
+    <t>Áo thun BB - M</t>
+  </si>
+  <si>
+    <t>Áo thun</t>
+  </si>
+  <si>
+    <t>Quần tây BB - L</t>
+  </si>
+  <si>
+    <t>Quần tây</t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+  <si>
+    <t>Có</t>
+  </si>
+  <si>
+    <t>Không</t>
   </si>
 </sst>
 </file>
@@ -413,15 +437,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
@@ -481,18 +505,138 @@
         <v>10</v>
       </c>
     </row>
+    <row r="2" spans="1:15">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2">
+        <v>400000</v>
+      </c>
+      <c r="D2">
+        <v>200000</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>100</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <v>400000</v>
+      </c>
+      <c r="D3">
+        <v>200000</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>100</v>
+      </c>
+      <c r="L3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4">
+        <v>500000</v>
+      </c>
+      <c r="D4">
+        <v>400000</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>100</v>
+      </c>
+      <c r="L4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O4">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1000">
       <formula1>ListProducerNames</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H1001 L2:M1001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1000 M4:M1000">
       <formula1>"0,1"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1000">
       <formula1>"0,5,10"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1000">
       <formula1>ListProductGroupNames</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>